<commit_message>
契約手続き一覧 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/已完成/test_ホワイトボート_問い合わせ履歴.xlsx
+++ b/test_物件管理/已完成/test_ホワイトボート_問い合わせ履歴.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -3104,7 +3104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BW125"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -12470,7 +12470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>